<commit_message>
Add report pdf file
</commit_message>
<xml_diff>
--- a/WBS-14520464-15520621-Hoàng-Trọng-Duy-LInh_DangXuanPhong.xlsx
+++ b/WBS-14520464-15520621-Hoàng-Trọng-Duy-LInh_DangXuanPhong.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HOCKY7\IS208\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HOCKY7\IS208\QLDA_IS208\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>Chi Phí (VNĐ)</t>
-  </si>
-  <si>
-    <t>Hệ thống quản lý quán cà phê Will Coffee</t>
   </si>
   <si>
     <t>1. Công tác chuẩn bị</t>
@@ -343,6 +340,9 @@
   </si>
   <si>
     <t>4.5. Test sự hài lòng của giáo viên</t>
+  </si>
+  <si>
+    <t>Hệ thống quản lý học sinh THPT Lê Quý Đôn</t>
   </si>
 </sst>
 </file>
@@ -937,6 +937,80 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -961,85 +1035,11 @@
     <xf numFmtId="1" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1370,8 +1370,8 @@
   </sheetPr>
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="B67" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1387,13 +1387,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="16.5">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="67" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1431,7 +1431,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="C2" s="66">
         <f>SUM(C3,C9,C19,C61,C68,C74,C77,C80)</f>
@@ -1472,7 +1472,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="68">
         <f>SUM(C4:C8)</f>
@@ -1485,7 +1485,7 @@
         <v>43393</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G3" s="36">
         <f>SUM(G4:G8)</f>
@@ -1515,7 +1515,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="66">
         <v>2</v>
@@ -1527,7 +1527,7 @@
         <v>43385</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" s="11">
         <v>0</v>
@@ -1556,7 +1556,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="66">
         <v>2</v>
@@ -1568,7 +1568,7 @@
         <v>43386</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G5" s="11">
         <v>0</v>
@@ -1597,7 +1597,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="66">
         <v>2</v>
@@ -1608,8 +1608,8 @@
       <c r="E6" s="14">
         <v>43388</v>
       </c>
-      <c r="F6" s="109" t="s">
-        <v>63</v>
+      <c r="F6" s="100" t="s">
+        <v>62</v>
       </c>
       <c r="G6" s="11">
         <v>0</v>
@@ -1638,7 +1638,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="66">
         <v>2</v>
@@ -1649,7 +1649,7 @@
       <c r="E7" s="14">
         <v>43392</v>
       </c>
-      <c r="F7" s="101"/>
+      <c r="F7" s="92"/>
       <c r="G7" s="11">
         <v>100000</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="66">
         <v>2</v>
@@ -1689,7 +1689,7 @@
         <v>43393</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G8" s="11">
         <v>400000</v>
@@ -1718,7 +1718,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="69">
         <f>SUM(C10:C18)</f>
@@ -1730,8 +1730,8 @@
       <c r="E9" s="34">
         <v>43418</v>
       </c>
-      <c r="F9" s="111" t="s">
-        <v>65</v>
+      <c r="F9" s="101" t="s">
+        <v>64</v>
       </c>
       <c r="G9" s="36">
         <f>SUM(G10:G18)</f>
@@ -1761,7 +1761,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="66">
         <v>8</v>
@@ -1772,7 +1772,7 @@
       <c r="E10" s="14">
         <v>43395</v>
       </c>
-      <c r="F10" s="99"/>
+      <c r="F10" s="96"/>
       <c r="G10" s="11">
         <v>100000</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="66">
         <v>2</v>
@@ -1811,7 +1811,7 @@
       <c r="E11" s="13">
         <v>43396</v>
       </c>
-      <c r="F11" s="99"/>
+      <c r="F11" s="96"/>
       <c r="G11" s="11">
         <v>50000</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="66">
         <v>2</v>
@@ -1850,7 +1850,7 @@
       <c r="E12" s="13">
         <v>43397</v>
       </c>
-      <c r="F12" s="99"/>
+      <c r="F12" s="96"/>
       <c r="G12" s="11">
         <v>50000</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="66">
         <v>8</v>
@@ -1889,7 +1889,7 @@
       <c r="E13" s="13">
         <v>43400</v>
       </c>
-      <c r="F13" s="99"/>
+      <c r="F13" s="96"/>
       <c r="G13" s="11">
         <v>50000</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="66">
         <v>8</v>
@@ -1928,7 +1928,7 @@
       <c r="E14" s="13">
         <v>43403</v>
       </c>
-      <c r="F14" s="99"/>
+      <c r="F14" s="96"/>
       <c r="G14" s="11">
         <v>50000</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="66">
         <v>8</v>
@@ -1967,7 +1967,7 @@
       <c r="E15" s="13">
         <v>43406</v>
       </c>
-      <c r="F15" s="99"/>
+      <c r="F15" s="96"/>
       <c r="G15" s="11">
         <v>50000</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="66">
         <v>2</v>
@@ -2006,7 +2006,7 @@
       <c r="E16" s="13">
         <v>43409</v>
       </c>
-      <c r="F16" s="99"/>
+      <c r="F16" s="96"/>
       <c r="G16" s="11">
         <v>50000</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="66">
         <v>2</v>
@@ -2045,7 +2045,7 @@
       <c r="E17" s="13">
         <v>43415</v>
       </c>
-      <c r="F17" s="99"/>
+      <c r="F17" s="96"/>
       <c r="G17" s="11">
         <v>50000</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="66">
         <v>2</v>
@@ -2084,7 +2084,7 @@
       <c r="E18" s="13">
         <v>43418</v>
       </c>
-      <c r="F18" s="99"/>
+      <c r="F18" s="96"/>
       <c r="G18" s="11">
         <v>50000</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="69">
         <f>SUM(C20,C22,C41,C42)</f>
@@ -2125,7 +2125,7 @@
         <v>43449</v>
       </c>
       <c r="F19" s="32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G19" s="60">
         <f>SUM(G20,G22,G41,G42)</f>
@@ -2155,7 +2155,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="70">
         <v>8</v>
@@ -2166,8 +2166,8 @@
       <c r="E20" s="13">
         <v>43420</v>
       </c>
-      <c r="F20" s="107" t="s">
-        <v>68</v>
+      <c r="F20" s="114" t="s">
+        <v>67</v>
       </c>
       <c r="G20" s="61">
         <v>800000</v>
@@ -2196,7 +2196,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="66">
         <v>8</v>
@@ -2207,7 +2207,7 @@
       <c r="E21" s="13">
         <v>43420</v>
       </c>
-      <c r="F21" s="99"/>
+      <c r="F21" s="96"/>
       <c r="G21" s="62">
         <v>800000</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="75">
         <f>SUM(C23,C24,C25,C26,C38)</f>
@@ -2249,7 +2249,7 @@
         <v>43432</v>
       </c>
       <c r="F22" s="58" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G22" s="59">
         <f>SUM(G23,G25,G26,G38)</f>
@@ -2280,21 +2280,21 @@
         <v>22</v>
       </c>
       <c r="B23" s="74" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="77">
         <v>24</v>
       </c>
-      <c r="D23" s="114">
+      <c r="D23" s="109">
         <v>43421</v>
       </c>
-      <c r="E23" s="103">
+      <c r="E23" s="91">
         <v>43452</v>
       </c>
-      <c r="F23" s="112" t="s">
-        <v>68</v>
-      </c>
-      <c r="G23" s="110">
+      <c r="F23" s="107" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="93">
         <v>5000000</v>
       </c>
       <c r="H23" s="15"/>
@@ -2322,15 +2322,15 @@
         <v>23</v>
       </c>
       <c r="B24" s="74" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="78">
         <v>8</v>
       </c>
-      <c r="D24" s="115"/>
-      <c r="E24" s="101"/>
-      <c r="F24" s="113"/>
-      <c r="G24" s="101"/>
+      <c r="D24" s="110"/>
+      <c r="E24" s="92"/>
+      <c r="F24" s="108"/>
+      <c r="G24" s="92"/>
       <c r="H24" s="15"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
@@ -2354,7 +2354,7 @@
     <row r="25" spans="1:26" ht="16.5">
       <c r="A25" s="6"/>
       <c r="B25" s="74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C25" s="78">
         <v>16</v>
@@ -2394,7 +2394,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" s="76">
         <f>SUM(C27,C30,C33,C35,C38)</f>
@@ -2407,7 +2407,7 @@
         <v>43432</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G26" s="11">
         <f>SUM(G27,G30,G33,G35)</f>
@@ -2438,21 +2438,21 @@
         <v>25</v>
       </c>
       <c r="B27" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="102">
+        <v>75</v>
+      </c>
+      <c r="C27" s="98">
         <v>12</v>
       </c>
-      <c r="D27" s="103">
+      <c r="D27" s="91">
         <v>43425</v>
       </c>
-      <c r="E27" s="103">
+      <c r="E27" s="91">
         <v>43425</v>
       </c>
-      <c r="F27" s="100" t="s">
-        <v>63</v>
-      </c>
-      <c r="G27" s="110">
+      <c r="F27" s="97" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" s="93">
         <v>6000000</v>
       </c>
       <c r="H27" s="15"/>
@@ -2480,13 +2480,13 @@
         <v>26</v>
       </c>
       <c r="B28" s="45" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" s="120"/>
-      <c r="D28" s="118"/>
-      <c r="E28" s="118"/>
-      <c r="F28" s="98"/>
-      <c r="G28" s="116"/>
+        <v>76</v>
+      </c>
+      <c r="C28" s="102"/>
+      <c r="D28" s="104"/>
+      <c r="E28" s="104"/>
+      <c r="F28" s="124"/>
+      <c r="G28" s="94"/>
       <c r="H28" s="15"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
@@ -2512,13 +2512,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="44" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="121"/>
-      <c r="D29" s="119"/>
-      <c r="E29" s="119"/>
-      <c r="F29" s="117"/>
-      <c r="G29" s="122"/>
+        <v>77</v>
+      </c>
+      <c r="C29" s="103"/>
+      <c r="D29" s="105"/>
+      <c r="E29" s="105"/>
+      <c r="F29" s="125"/>
+      <c r="G29" s="95"/>
       <c r="H29" s="15"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
@@ -2544,21 +2544,21 @@
         <v>28</v>
       </c>
       <c r="B30" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="C30" s="102">
+        <v>78</v>
+      </c>
+      <c r="C30" s="98">
         <v>12</v>
       </c>
-      <c r="D30" s="103">
+      <c r="D30" s="91">
         <v>43426</v>
       </c>
-      <c r="E30" s="103">
+      <c r="E30" s="91">
         <v>43426</v>
       </c>
-      <c r="F30" s="100" t="s">
-        <v>64</v>
-      </c>
-      <c r="G30" s="110">
+      <c r="F30" s="97" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="93">
         <v>6000000</v>
       </c>
       <c r="H30" s="15"/>
@@ -2586,13 +2586,13 @@
         <v>29</v>
       </c>
       <c r="B31" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="96"/>
-      <c r="D31" s="99"/>
-      <c r="E31" s="99"/>
-      <c r="F31" s="99"/>
-      <c r="G31" s="99"/>
+        <v>79</v>
+      </c>
+      <c r="C31" s="106"/>
+      <c r="D31" s="96"/>
+      <c r="E31" s="96"/>
+      <c r="F31" s="96"/>
+      <c r="G31" s="96"/>
       <c r="H31" s="15"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
@@ -2618,13 +2618,13 @@
         <v>30</v>
       </c>
       <c r="B32" s="44" t="s">
-        <v>81</v>
-      </c>
-      <c r="C32" s="97"/>
-      <c r="D32" s="101"/>
-      <c r="E32" s="101"/>
-      <c r="F32" s="99"/>
-      <c r="G32" s="101"/>
+        <v>80</v>
+      </c>
+      <c r="C32" s="99"/>
+      <c r="D32" s="92"/>
+      <c r="E32" s="92"/>
+      <c r="F32" s="96"/>
+      <c r="G32" s="92"/>
       <c r="H32" s="15"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
@@ -2650,19 +2650,19 @@
         <v>31</v>
       </c>
       <c r="B33" s="44" t="s">
-        <v>82</v>
-      </c>
-      <c r="C33" s="102">
+        <v>81</v>
+      </c>
+      <c r="C33" s="98">
         <v>12</v>
       </c>
-      <c r="D33" s="103">
+      <c r="D33" s="91">
         <v>43427</v>
       </c>
-      <c r="E33" s="103">
+      <c r="E33" s="91">
         <v>43427</v>
       </c>
-      <c r="F33" s="99"/>
-      <c r="G33" s="110">
+      <c r="F33" s="96"/>
+      <c r="G33" s="93">
         <v>4000000</v>
       </c>
       <c r="H33" s="15"/>
@@ -2690,13 +2690,13 @@
         <v>32</v>
       </c>
       <c r="B34" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="C34" s="97"/>
-      <c r="D34" s="101"/>
-      <c r="E34" s="101"/>
-      <c r="F34" s="99"/>
-      <c r="G34" s="101"/>
+        <v>82</v>
+      </c>
+      <c r="C34" s="99"/>
+      <c r="D34" s="92"/>
+      <c r="E34" s="92"/>
+      <c r="F34" s="96"/>
+      <c r="G34" s="92"/>
       <c r="H34" s="15"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
@@ -2722,7 +2722,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C35" s="71">
         <f>SUM(C36:C37)</f>
@@ -2734,7 +2734,7 @@
       <c r="E35" s="14">
         <v>43429</v>
       </c>
-      <c r="F35" s="101"/>
+      <c r="F35" s="92"/>
       <c r="G35" s="11">
         <f>SUM(G36:G37)</f>
         <v>4000000</v>
@@ -2764,7 +2764,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C36" s="66">
         <v>8</v>
@@ -2775,8 +2775,8 @@
       <c r="E36" s="14">
         <v>43428</v>
       </c>
-      <c r="F36" s="100" t="s">
-        <v>69</v>
+      <c r="F36" s="97" t="s">
+        <v>68</v>
       </c>
       <c r="G36" s="11">
         <v>2000000</v>
@@ -2806,7 +2806,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C37" s="66">
         <v>8</v>
@@ -2817,7 +2817,7 @@
       <c r="E37" s="14">
         <v>43429</v>
       </c>
-      <c r="F37" s="99"/>
+      <c r="F37" s="96"/>
       <c r="G37" s="11">
         <v>2000000</v>
       </c>
@@ -2846,19 +2846,19 @@
         <v>36</v>
       </c>
       <c r="B38" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="C38" s="95">
+        <v>28</v>
+      </c>
+      <c r="C38" s="123">
         <v>8</v>
       </c>
-      <c r="D38" s="103">
+      <c r="D38" s="91">
         <v>43430</v>
       </c>
-      <c r="E38" s="103">
+      <c r="E38" s="91">
         <v>43432</v>
       </c>
-      <c r="F38" s="99"/>
-      <c r="G38" s="110">
+      <c r="F38" s="96"/>
+      <c r="G38" s="93">
         <v>4000000</v>
       </c>
       <c r="H38" s="15"/>
@@ -2886,13 +2886,13 @@
         <v>37</v>
       </c>
       <c r="B39" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="C39" s="96"/>
-      <c r="D39" s="99"/>
-      <c r="E39" s="99"/>
-      <c r="F39" s="99"/>
-      <c r="G39" s="99"/>
+        <v>29</v>
+      </c>
+      <c r="C39" s="106"/>
+      <c r="D39" s="96"/>
+      <c r="E39" s="96"/>
+      <c r="F39" s="96"/>
+      <c r="G39" s="96"/>
       <c r="H39" s="15"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
@@ -2918,13 +2918,13 @@
         <v>38</v>
       </c>
       <c r="B40" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" s="97"/>
-      <c r="D40" s="101"/>
-      <c r="E40" s="101"/>
-      <c r="F40" s="101"/>
-      <c r="G40" s="101"/>
+        <v>30</v>
+      </c>
+      <c r="C40" s="99"/>
+      <c r="D40" s="92"/>
+      <c r="E40" s="92"/>
+      <c r="F40" s="92"/>
+      <c r="G40" s="92"/>
       <c r="H40" s="15"/>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
@@ -2950,7 +2950,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="51" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C41" s="72">
         <v>8</v>
@@ -2962,7 +2962,7 @@
         <v>43432</v>
       </c>
       <c r="F41" s="52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G41" s="53">
         <v>200000</v>
@@ -2992,7 +2992,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="51" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C42" s="72">
         <f>SUM(C43,C48)</f>
@@ -3005,7 +3005,7 @@
         <v>43451</v>
       </c>
       <c r="F42" s="54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G42" s="53">
         <f>SUM(G43,G48)</f>
@@ -3035,7 +3035,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C43" s="71">
         <v>8</v>
@@ -3046,10 +3046,10 @@
       <c r="E43" s="14">
         <v>43437</v>
       </c>
-      <c r="F43" s="100" t="s">
-        <v>63</v>
-      </c>
-      <c r="G43" s="110">
+      <c r="F43" s="97" t="s">
+        <v>62</v>
+      </c>
+      <c r="G43" s="93">
         <v>15000000</v>
       </c>
       <c r="I43" s="5"/>
@@ -3076,9 +3076,9 @@
         <v>42</v>
       </c>
       <c r="B44" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="C44" s="92">
+        <v>34</v>
+      </c>
+      <c r="C44" s="120">
         <v>8</v>
       </c>
       <c r="D44" s="14">
@@ -3087,8 +3087,8 @@
       <c r="E44" s="14">
         <v>43433</v>
       </c>
-      <c r="F44" s="99"/>
-      <c r="G44" s="99"/>
+      <c r="F44" s="96"/>
+      <c r="G44" s="96"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
       <c r="K44" s="5"/>
@@ -3113,17 +3113,17 @@
         <v>43</v>
       </c>
       <c r="B45" s="47" t="s">
-        <v>75</v>
-      </c>
-      <c r="C45" s="93"/>
+        <v>74</v>
+      </c>
+      <c r="C45" s="121"/>
       <c r="D45" s="14">
         <v>43434</v>
       </c>
       <c r="E45" s="14">
         <v>43434</v>
       </c>
-      <c r="F45" s="99"/>
-      <c r="G45" s="99"/>
+      <c r="F45" s="96"/>
+      <c r="G45" s="96"/>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
@@ -3148,17 +3148,17 @@
         <v>44</v>
       </c>
       <c r="B46" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="C46" s="93"/>
+        <v>35</v>
+      </c>
+      <c r="C46" s="121"/>
       <c r="D46" s="14">
         <v>43405</v>
       </c>
       <c r="E46" s="14">
         <v>43405</v>
       </c>
-      <c r="F46" s="99"/>
-      <c r="G46" s="99"/>
+      <c r="F46" s="96"/>
+      <c r="G46" s="96"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
       <c r="K46" s="5"/>
@@ -3183,17 +3183,17 @@
         <v>45</v>
       </c>
       <c r="B47" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="C47" s="94"/>
+        <v>36</v>
+      </c>
+      <c r="C47" s="122"/>
       <c r="D47" s="14">
         <v>43436</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="F47" s="99"/>
-      <c r="G47" s="101"/>
+        <v>61</v>
+      </c>
+      <c r="F47" s="96"/>
+      <c r="G47" s="92"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
@@ -3218,7 +3218,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C48" s="71">
         <f>SUM(C49:C60,)</f>
@@ -3230,8 +3230,8 @@
       <c r="E48" s="13">
         <v>43449</v>
       </c>
-      <c r="F48" s="108" t="s">
-        <v>70</v>
+      <c r="F48" s="115" t="s">
+        <v>69</v>
       </c>
       <c r="G48" s="11">
         <f>SUM(G49,G50)</f>
@@ -3261,7 +3261,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="47" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C49" s="71">
         <v>4</v>
@@ -3272,7 +3272,7 @@
       <c r="E49" s="14">
         <v>43438</v>
       </c>
-      <c r="F49" s="99"/>
+      <c r="F49" s="96"/>
       <c r="G49" s="11">
         <v>400000</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="47" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C50" s="71">
         <f>SUM(C51:C52)</f>
@@ -3312,7 +3312,7 @@
       <c r="E50" s="29">
         <v>43443</v>
       </c>
-      <c r="F50" s="99"/>
+      <c r="F50" s="96"/>
       <c r="G50" s="11">
         <f>SUM(G51:G60)</f>
         <v>48000000</v>
@@ -3341,7 +3341,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C51" s="66">
         <v>8</v>
@@ -3352,7 +3352,7 @@
       <c r="E51" s="14">
         <v>43440</v>
       </c>
-      <c r="F51" s="99"/>
+      <c r="F51" s="96"/>
       <c r="G51" s="11">
         <v>12000000</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C52" s="66">
         <v>8</v>
@@ -3391,7 +3391,7 @@
       <c r="E52" s="29">
         <v>43442</v>
       </c>
-      <c r="F52" s="101"/>
+      <c r="F52" s="92"/>
       <c r="G52" s="11">
         <v>13000000</v>
       </c>
@@ -3418,22 +3418,22 @@
       <c r="A53" s="6">
         <v>52</v>
       </c>
-      <c r="B53" s="123" t="s">
-        <v>90</v>
-      </c>
-      <c r="C53" s="102">
+      <c r="B53" s="88" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" s="98">
         <v>8</v>
       </c>
-      <c r="D53" s="103">
+      <c r="D53" s="91">
         <v>43444</v>
       </c>
-      <c r="E53" s="103">
+      <c r="E53" s="91">
         <v>43444</v>
       </c>
-      <c r="F53" s="98" t="s">
-        <v>63</v>
-      </c>
-      <c r="G53" s="110">
+      <c r="F53" s="124" t="s">
+        <v>62</v>
+      </c>
+      <c r="G53" s="93">
         <v>18000000</v>
       </c>
       <c r="I53" s="5"/>
@@ -3459,14 +3459,14 @@
       <c r="A54" s="6">
         <v>53</v>
       </c>
-      <c r="B54" s="124" t="s">
-        <v>91</v>
-      </c>
-      <c r="C54" s="97"/>
-      <c r="D54" s="101"/>
-      <c r="E54" s="101"/>
-      <c r="F54" s="99"/>
-      <c r="G54" s="99"/>
+      <c r="B54" s="89" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54" s="99"/>
+      <c r="D54" s="92"/>
+      <c r="E54" s="92"/>
+      <c r="F54" s="96"/>
+      <c r="G54" s="96"/>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
@@ -3490,20 +3490,20 @@
       <c r="A55" s="6">
         <v>54</v>
       </c>
-      <c r="B55" s="123" t="s">
-        <v>92</v>
-      </c>
-      <c r="C55" s="102">
+      <c r="B55" s="88" t="s">
+        <v>91</v>
+      </c>
+      <c r="C55" s="98">
         <v>8</v>
       </c>
-      <c r="D55" s="103">
+      <c r="D55" s="91">
         <v>43445</v>
       </c>
-      <c r="E55" s="103">
+      <c r="E55" s="91">
         <v>43445</v>
       </c>
-      <c r="F55" s="99"/>
-      <c r="G55" s="99"/>
+      <c r="F55" s="96"/>
+      <c r="G55" s="96"/>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
       <c r="K55" s="5"/>
@@ -3527,14 +3527,14 @@
       <c r="A56" s="6">
         <v>55</v>
       </c>
-      <c r="B56" s="123" t="s">
-        <v>93</v>
-      </c>
-      <c r="C56" s="97"/>
-      <c r="D56" s="101"/>
-      <c r="E56" s="101"/>
-      <c r="F56" s="99"/>
-      <c r="G56" s="99"/>
+      <c r="B56" s="88" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" s="99"/>
+      <c r="D56" s="92"/>
+      <c r="E56" s="92"/>
+      <c r="F56" s="96"/>
+      <c r="G56" s="96"/>
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
       <c r="K56" s="5"/>
@@ -3558,20 +3558,20 @@
       <c r="A57" s="6">
         <v>56</v>
       </c>
-      <c r="B57" s="124" t="s">
-        <v>94</v>
-      </c>
-      <c r="C57" s="102">
+      <c r="B57" s="89" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57" s="98">
         <v>8</v>
       </c>
-      <c r="D57" s="103">
+      <c r="D57" s="91">
         <v>43446</v>
       </c>
-      <c r="E57" s="103">
+      <c r="E57" s="91">
         <v>43446</v>
       </c>
-      <c r="F57" s="99"/>
-      <c r="G57" s="99"/>
+      <c r="F57" s="96"/>
+      <c r="G57" s="96"/>
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
@@ -3595,14 +3595,14 @@
       <c r="A58" s="6">
         <v>57</v>
       </c>
-      <c r="B58" s="123" t="s">
-        <v>95</v>
-      </c>
-      <c r="C58" s="97"/>
-      <c r="D58" s="101"/>
-      <c r="E58" s="101"/>
-      <c r="F58" s="101"/>
-      <c r="G58" s="101"/>
+      <c r="B58" s="88" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="99"/>
+      <c r="D58" s="92"/>
+      <c r="E58" s="92"/>
+      <c r="F58" s="92"/>
+      <c r="G58" s="92"/>
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
       <c r="K58" s="5"/>
@@ -3626,8 +3626,8 @@
       <c r="A59" s="6">
         <v>58</v>
       </c>
-      <c r="B59" s="123" t="s">
-        <v>96</v>
+      <c r="B59" s="88" t="s">
+        <v>95</v>
       </c>
       <c r="C59" s="66">
         <v>4</v>
@@ -3638,10 +3638,10 @@
       <c r="E59" s="13">
         <v>43447</v>
       </c>
-      <c r="F59" s="100" t="s">
-        <v>64</v>
-      </c>
-      <c r="G59" s="110">
+      <c r="F59" s="97" t="s">
+        <v>63</v>
+      </c>
+      <c r="G59" s="93">
         <v>5000000</v>
       </c>
       <c r="I59" s="5"/>
@@ -3667,8 +3667,8 @@
       <c r="A60" s="6">
         <v>59</v>
       </c>
-      <c r="B60" s="123" t="s">
-        <v>97</v>
+      <c r="B60" s="88" t="s">
+        <v>96</v>
       </c>
       <c r="C60" s="66">
         <v>4</v>
@@ -3679,8 +3679,8 @@
       <c r="E60" s="13">
         <v>43448</v>
       </c>
-      <c r="F60" s="101"/>
-      <c r="G60" s="101"/>
+      <c r="F60" s="92"/>
+      <c r="G60" s="92"/>
       <c r="I60" s="5"/>
       <c r="J60" s="5"/>
       <c r="K60" s="5"/>
@@ -3705,7 +3705,7 @@
         <v>63</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C61" s="73">
         <f>SUM(C62:C67)</f>
@@ -3717,8 +3717,8 @@
       <c r="E61" s="18">
         <v>43461</v>
       </c>
-      <c r="F61" s="100" t="s">
-        <v>68</v>
+      <c r="F61" s="97" t="s">
+        <v>67</v>
       </c>
       <c r="G61" s="9">
         <f>SUM(G62:G67)</f>
@@ -3749,7 +3749,7 @@
         <v>64</v>
       </c>
       <c r="B62" s="40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C62" s="66">
         <v>2</v>
@@ -3760,7 +3760,7 @@
       <c r="E62" s="13">
         <v>43452</v>
       </c>
-      <c r="F62" s="99"/>
+      <c r="F62" s="96"/>
       <c r="G62" s="11">
         <v>1000000</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>65</v>
       </c>
       <c r="B63" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C63" s="66">
         <v>2</v>
@@ -3800,7 +3800,7 @@
       <c r="E63" s="13">
         <v>43453</v>
       </c>
-      <c r="F63" s="101"/>
+      <c r="F63" s="92"/>
       <c r="G63" s="11">
         <v>1000000</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>66</v>
       </c>
       <c r="B64" s="40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C64" s="66">
         <v>16</v>
@@ -3840,10 +3840,10 @@
       <c r="E64" s="13">
         <v>43454</v>
       </c>
-      <c r="F64" s="100" t="s">
-        <v>74</v>
-      </c>
-      <c r="G64" s="110">
+      <c r="F64" s="97" t="s">
+        <v>73</v>
+      </c>
+      <c r="G64" s="93">
         <v>12000000</v>
       </c>
       <c r="H64" s="19"/>
@@ -3871,7 +3871,7 @@
         <v>67</v>
       </c>
       <c r="B65" s="39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C65" s="66">
         <v>16</v>
@@ -3882,8 +3882,8 @@
       <c r="E65" s="13">
         <v>43455</v>
       </c>
-      <c r="F65" s="99"/>
-      <c r="G65" s="99"/>
+      <c r="F65" s="96"/>
+      <c r="G65" s="96"/>
       <c r="H65" s="19"/>
       <c r="I65" s="20"/>
       <c r="J65" s="20"/>
@@ -3908,8 +3908,8 @@
       <c r="A66" s="6">
         <v>68</v>
       </c>
-      <c r="B66" s="125" t="s">
-        <v>98</v>
+      <c r="B66" s="90" t="s">
+        <v>97</v>
       </c>
       <c r="C66" s="71">
         <v>8</v>
@@ -3920,8 +3920,8 @@
       <c r="E66" s="13">
         <v>43457</v>
       </c>
-      <c r="F66" s="101"/>
-      <c r="G66" s="101"/>
+      <c r="F66" s="92"/>
+      <c r="G66" s="92"/>
       <c r="H66" s="19"/>
       <c r="I66" s="20"/>
       <c r="J66" s="20"/>
@@ -3947,7 +3947,7 @@
         <v>69</v>
       </c>
       <c r="B67" s="39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C67" s="66">
         <v>8</v>
@@ -3959,7 +3959,7 @@
         <v>43461</v>
       </c>
       <c r="F67" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G67" s="11">
         <v>1000000</v>
@@ -3989,7 +3989,7 @@
         <v>70</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C68" s="73">
         <f>SUM(C69:C73)</f>
@@ -4001,8 +4001,8 @@
       <c r="E68" s="18">
         <v>43106</v>
       </c>
-      <c r="F68" s="108" t="s">
-        <v>71</v>
+      <c r="F68" s="115" t="s">
+        <v>70</v>
       </c>
       <c r="G68" s="9">
         <f>SUM(G69:G73)</f>
@@ -4033,7 +4033,7 @@
         <v>71</v>
       </c>
       <c r="B69" s="40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C69" s="66">
         <v>8</v>
@@ -4044,7 +4044,7 @@
       <c r="E69" s="13">
         <v>43463</v>
       </c>
-      <c r="F69" s="99"/>
+      <c r="F69" s="96"/>
       <c r="G69" s="11">
         <v>2000000</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>72</v>
       </c>
       <c r="B70" s="40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C70" s="66">
         <v>8</v>
@@ -4084,7 +4084,7 @@
       <c r="E70" s="13">
         <v>43830</v>
       </c>
-      <c r="F70" s="99"/>
+      <c r="F70" s="96"/>
       <c r="G70" s="11">
         <v>2000000</v>
       </c>
@@ -4113,7 +4113,7 @@
         <v>73</v>
       </c>
       <c r="B71" s="40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C71" s="66">
         <v>8</v>
@@ -4124,7 +4124,7 @@
       <c r="E71" s="13">
         <v>43467</v>
       </c>
-      <c r="F71" s="99"/>
+      <c r="F71" s="96"/>
       <c r="G71" s="10">
         <v>0</v>
       </c>
@@ -4153,7 +4153,7 @@
         <v>74</v>
       </c>
       <c r="B72" s="40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C72" s="66">
         <v>8</v>
@@ -4164,7 +4164,7 @@
       <c r="E72" s="13">
         <v>43468</v>
       </c>
-      <c r="F72" s="99"/>
+      <c r="F72" s="96"/>
       <c r="G72" s="11">
         <v>2000000</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>75</v>
       </c>
       <c r="B73" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C73" s="66">
         <v>8</v>
@@ -4204,7 +4204,7 @@
       <c r="E73" s="13">
         <v>43470</v>
       </c>
-      <c r="F73" s="101"/>
+      <c r="F73" s="92"/>
       <c r="G73" s="10">
         <v>0</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>76</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C74" s="73">
         <f>SUM(C76,C75)</f>
@@ -4245,8 +4245,8 @@
       <c r="E74" s="18">
         <v>43474</v>
       </c>
-      <c r="F74" s="108" t="s">
-        <v>66</v>
+      <c r="F74" s="115" t="s">
+        <v>65</v>
       </c>
       <c r="G74" s="9">
         <f>SUM(G75,G76)</f>
@@ -4277,7 +4277,7 @@
         <v>77</v>
       </c>
       <c r="B75" s="40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C75" s="66">
         <v>2</v>
@@ -4288,7 +4288,7 @@
       <c r="E75" s="13">
         <v>43471</v>
       </c>
-      <c r="F75" s="99"/>
+      <c r="F75" s="96"/>
       <c r="G75" s="22">
         <v>0</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>78</v>
       </c>
       <c r="B76" s="40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C76" s="66">
         <v>8</v>
@@ -4328,7 +4328,7 @@
       <c r="E76" s="13">
         <v>43474</v>
       </c>
-      <c r="F76" s="101"/>
+      <c r="F76" s="92"/>
       <c r="G76" s="28">
         <v>2000000</v>
       </c>
@@ -4357,7 +4357,7 @@
         <v>79</v>
       </c>
       <c r="B77" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C77" s="73">
         <f>SUM(C78:C79)</f>
@@ -4369,8 +4369,8 @@
       <c r="E77" s="18">
         <v>43475</v>
       </c>
-      <c r="F77" s="104" t="s">
-        <v>69</v>
+      <c r="F77" s="111" t="s">
+        <v>68</v>
       </c>
       <c r="G77" s="65">
         <f>SUM(G78:G79)</f>
@@ -4401,7 +4401,7 @@
         <v>80</v>
       </c>
       <c r="B78" s="40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C78" s="66">
         <v>0</v>
@@ -4412,7 +4412,7 @@
       <c r="E78" s="23">
         <v>43475</v>
       </c>
-      <c r="F78" s="105"/>
+      <c r="F78" s="112"/>
       <c r="G78" s="64">
         <v>0</v>
       </c>
@@ -4441,7 +4441,7 @@
         <v>81</v>
       </c>
       <c r="B79" s="40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C79" s="66">
         <v>0</v>
@@ -4452,7 +4452,7 @@
       <c r="E79" s="23">
         <v>43475</v>
       </c>
-      <c r="F79" s="106"/>
+      <c r="F79" s="113"/>
       <c r="G79" s="64">
         <v>0</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>82</v>
       </c>
       <c r="B80" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C80" s="73">
         <v>0</v>
@@ -4493,7 +4493,7 @@
         <v>43809</v>
       </c>
       <c r="F80" s="81" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G80" s="63">
         <v>0</v>
@@ -4520,12 +4520,12 @@
     </row>
     <row r="81" spans="1:26" ht="16.5">
       <c r="A81" s="25"/>
-      <c r="B81" s="88"/>
+      <c r="B81" s="116"/>
       <c r="C81" s="79"/>
       <c r="D81" s="5"/>
       <c r="E81" s="5"/>
       <c r="F81" s="26"/>
-      <c r="G81" s="90"/>
+      <c r="G81" s="118"/>
       <c r="I81" s="5"/>
       <c r="J81" s="5"/>
       <c r="K81" s="5"/>
@@ -4547,12 +4547,12 @@
     </row>
     <row r="82" spans="1:26" ht="16.5">
       <c r="A82" s="25"/>
-      <c r="B82" s="89"/>
+      <c r="B82" s="117"/>
       <c r="C82" s="79"/>
       <c r="D82" s="5"/>
       <c r="E82" s="5"/>
       <c r="F82" s="26"/>
-      <c r="G82" s="91"/>
+      <c r="G82" s="119"/>
       <c r="I82" s="5"/>
       <c r="J82" s="5"/>
       <c r="K82" s="5"/>
@@ -29144,41 +29144,6 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="G27:G29"/>
-    <mergeCell ref="G43:G47"/>
-    <mergeCell ref="G30:G32"/>
-    <mergeCell ref="G64:G66"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="F36:F40"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="G53:G58"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="F9:F18"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="F77:F79"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="F43:F47"/>
-    <mergeCell ref="F61:F63"/>
-    <mergeCell ref="F64:F66"/>
-    <mergeCell ref="F48:F52"/>
-    <mergeCell ref="F68:F73"/>
-    <mergeCell ref="F74:F76"/>
     <mergeCell ref="B81:B82"/>
     <mergeCell ref="G81:G82"/>
     <mergeCell ref="C44:C47"/>
@@ -29195,6 +29160,41 @@
     <mergeCell ref="D53:D54"/>
     <mergeCell ref="E53:E54"/>
     <mergeCell ref="D55:D56"/>
+    <mergeCell ref="F77:F79"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="F43:F47"/>
+    <mergeCell ref="F61:F63"/>
+    <mergeCell ref="F64:F66"/>
+    <mergeCell ref="F48:F52"/>
+    <mergeCell ref="F68:F73"/>
+    <mergeCell ref="F74:F76"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="F9:F18"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="G27:G29"/>
+    <mergeCell ref="G43:G47"/>
+    <mergeCell ref="G30:G32"/>
+    <mergeCell ref="G64:G66"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="F36:F40"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="G53:G58"/>
   </mergeCells>
   <conditionalFormatting sqref="J6:J11 L12">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">

</xml_diff>